<commit_message>
Update Factorial Analysis 3 repeat.xlsx
</commit_message>
<xml_diff>
--- a/analysis/analisiFattoriale-tmkX/Factorial Analysis 3 repeat.xlsx
+++ b/analysis/analisiFattoriale-tmkX/Factorial Analysis 3 repeat.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaia\Documents\GitHub\PECSNproject\analysis\analisiFattoriale-tmkX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756ED645-07F0-4551-93E6-CC4800EFBBB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DB04AB-9977-4111-AE71-36A49E1DEE04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C7BA823-641E-4C67-8975-4763F16E04BA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>t = ${0.5,2}s</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>SST</t>
+  </si>
+  <si>
+    <t>Variation (%)</t>
+  </si>
+  <si>
+    <t>Variation(%)</t>
   </si>
 </sst>
 </file>
@@ -157,7 +163,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -188,12 +194,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -511,21 +518,25 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25"/>
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
@@ -658,19 +669,19 @@
         <v>1.2366842845096E-2</v>
       </c>
       <c r="W3">
-        <f>(T3+U3+V3)/3</f>
+        <f t="shared" ref="W3:W18" si="0">(T3+U3+V3)/3</f>
         <v>1.2409250133942E-2</v>
       </c>
       <c r="X3" s="2">
-        <f>T3-W3</f>
+        <f t="shared" ref="X3:X18" si="1">T3-W3</f>
         <v>6.6767414870008701E-6</v>
       </c>
       <c r="Y3" s="2">
-        <f>U3-W3</f>
+        <f t="shared" ref="Y3:Y18" si="2">U3-W3</f>
         <v>3.5730547358999581E-5</v>
       </c>
       <c r="Z3" s="2">
-        <f>V3-W3</f>
+        <f t="shared" ref="Z3:Z18" si="3">V3-W3</f>
         <v>-4.2407288846000452E-5</v>
       </c>
     </row>
@@ -736,19 +747,19 @@
         <v>6.0034368876877998E-2</v>
       </c>
       <c r="W4">
-        <f>(T4+U4+V4)/3</f>
+        <f t="shared" si="0"/>
         <v>5.5217432291134995E-2</v>
       </c>
       <c r="X4" s="2">
-        <f>T4-W4</f>
+        <f t="shared" si="1"/>
         <v>9.6421225950900358E-4</v>
       </c>
       <c r="Y4" s="2">
-        <f>U4-W4</f>
+        <f t="shared" si="2"/>
         <v>-5.7811488452519932E-3</v>
       </c>
       <c r="Z4" s="2">
-        <f>V4-W4</f>
+        <f t="shared" si="3"/>
         <v>4.8169365857430035E-3</v>
       </c>
     </row>
@@ -814,19 +825,19 @@
         <v>0.77525619023754999</v>
       </c>
       <c r="W5">
-        <f>(T5+U5+V5)/3</f>
+        <f t="shared" si="0"/>
         <v>0.67068497809881322</v>
       </c>
       <c r="X5" s="2">
-        <f>T5-W5</f>
+        <f t="shared" si="1"/>
         <v>-6.0591280487763188E-2</v>
       </c>
       <c r="Y5" s="2">
-        <f>U5-W5</f>
+        <f t="shared" si="2"/>
         <v>-4.3979931650973247E-2</v>
       </c>
       <c r="Z5" s="2">
-        <f>V5-W5</f>
+        <f t="shared" si="3"/>
         <v>0.10457121213873677</v>
       </c>
     </row>
@@ -892,19 +903,19 @@
         <v>1.4948030445012001E-2</v>
       </c>
       <c r="W6">
-        <f>(T6+U6+V6)/3</f>
+        <f t="shared" si="0"/>
         <v>1.4267450520792667E-2</v>
       </c>
       <c r="X6" s="2">
-        <f>T6-W6</f>
+        <f t="shared" si="1"/>
         <v>-1.41659603046667E-4</v>
       </c>
       <c r="Y6" s="2">
-        <f>U6-W6</f>
+        <f t="shared" si="2"/>
         <v>-5.3892032117266661E-4</v>
       </c>
       <c r="Z6" s="2">
-        <f>V6-W6</f>
+        <f t="shared" si="3"/>
         <v>6.8057992421933361E-4</v>
       </c>
     </row>
@@ -970,19 +981,19 @@
         <v>7.9646723792000992E-3</v>
       </c>
       <c r="W7">
-        <f>(T7+U7+V7)/3</f>
+        <f t="shared" si="0"/>
         <v>7.9970270740044019E-3</v>
       </c>
       <c r="X7" s="2">
-        <f>T7-W7</f>
+        <f t="shared" si="1"/>
         <v>1.0076710344598602E-5</v>
       </c>
       <c r="Y7" s="2">
-        <f>U7-W7</f>
+        <f t="shared" si="2"/>
         <v>2.2277984459698891E-5</v>
       </c>
       <c r="Z7" s="2">
-        <f>V7-W7</f>
+        <f t="shared" si="3"/>
         <v>-3.2354694804302697E-5</v>
       </c>
     </row>
@@ -1045,19 +1056,19 @@
         <v>3.9222777139216999E-2</v>
       </c>
       <c r="W8">
-        <f>(T8+U8+V8)/3</f>
+        <f t="shared" si="0"/>
         <v>3.9744695511026336E-2</v>
       </c>
       <c r="X8" s="2">
-        <f>T8-W8</f>
+        <f t="shared" si="1"/>
         <v>7.0666389743866131E-4</v>
       </c>
       <c r="Y8" s="2">
-        <f>U8-W8</f>
+        <f t="shared" si="2"/>
         <v>-1.8474552562933871E-4</v>
       </c>
       <c r="Z8" s="2">
-        <f>V8-W8</f>
+        <f t="shared" si="3"/>
         <v>-5.2191837180933648E-4</v>
       </c>
     </row>
@@ -1120,19 +1131,19 @@
         <v>0.59046036659578005</v>
       </c>
       <c r="W9">
-        <f>(T9+U9+V9)/3</f>
+        <f t="shared" si="0"/>
         <v>0.66420550831640346</v>
       </c>
       <c r="X9" s="2">
-        <f>T9-W9</f>
+        <f t="shared" si="1"/>
         <v>6.1013647066896493E-2</v>
       </c>
       <c r="Y9" s="2">
-        <f>U9-W9</f>
+        <f t="shared" si="2"/>
         <v>1.2731494653726583E-2</v>
       </c>
       <c r="Z9" s="2">
-        <f>V9-W9</f>
+        <f t="shared" si="3"/>
         <v>-7.3745141720623408E-2</v>
       </c>
     </row>
@@ -1198,19 +1209,19 @@
         <v>8.3570422034003004E-3</v>
       </c>
       <c r="W10">
-        <f>(T10+U10+V10)/3</f>
+        <f t="shared" si="0"/>
         <v>8.3951273031728658E-3</v>
       </c>
       <c r="X10" s="2">
-        <f>T10-W10</f>
+        <f t="shared" si="1"/>
         <v>1.8289695803350159E-7</v>
       </c>
       <c r="Y10" s="2">
-        <f>U10-W10</f>
+        <f t="shared" si="2"/>
         <v>3.7902202814533645E-5</v>
       </c>
       <c r="Z10" s="2">
-        <f>V10-W10</f>
+        <f t="shared" si="3"/>
         <v>-3.8085099772565412E-5</v>
       </c>
     </row>
@@ -1276,19 +1287,19 @@
         <v>1.2074195198359E-2</v>
       </c>
       <c r="W11">
-        <f>(T11+U11+V11)/3</f>
+        <f t="shared" si="0"/>
         <v>1.2017681792796666E-2</v>
       </c>
       <c r="X11" s="2">
-        <f>T11-W11</f>
+        <f t="shared" si="1"/>
         <v>-3.683631979665633E-6</v>
       </c>
       <c r="Y11" s="2">
-        <f>U11-W11</f>
+        <f t="shared" si="2"/>
         <v>-5.2829773582665704E-5</v>
       </c>
       <c r="Z11" s="2">
-        <f>V11-W11</f>
+        <f t="shared" si="3"/>
         <v>5.6513405562334806E-5</v>
       </c>
     </row>
@@ -1354,19 +1365,19 @@
         <v>4.8828473236715998E-2</v>
       </c>
       <c r="W12">
-        <f>(T12+U12+V12)/3</f>
+        <f t="shared" si="0"/>
         <v>5.0822014899664002E-2</v>
       </c>
       <c r="X12" s="2">
-        <f>T12-W12</f>
+        <f t="shared" si="1"/>
         <v>7.5099874702599934E-4</v>
       </c>
       <c r="Y12" s="2">
-        <f>U12-W12</f>
+        <f t="shared" si="2"/>
         <v>1.2425429159219972E-3</v>
       </c>
       <c r="Z12" s="2">
-        <f>V12-W12</f>
+        <f t="shared" si="3"/>
         <v>-1.9935416629480035E-3</v>
       </c>
     </row>
@@ -1390,47 +1401,47 @@
         <v>-1</v>
       </c>
       <c r="I13">
-        <f>E13*F13</f>
+        <f t="shared" ref="I13:I18" si="4">E13*F13</f>
         <v>-1</v>
       </c>
       <c r="J13">
-        <f>E13*G13</f>
+        <f t="shared" ref="J13:J18" si="5">E13*G13</f>
         <v>1</v>
       </c>
       <c r="K13">
-        <f>E13*H13</f>
+        <f t="shared" ref="K13:K18" si="6">E13*H13</f>
         <v>-1</v>
       </c>
       <c r="L13">
-        <f>F13*G13</f>
+        <f t="shared" ref="L13:L18" si="7">F13*G13</f>
         <v>-1</v>
       </c>
       <c r="M13">
-        <f>F13*H13</f>
+        <f t="shared" ref="M13:M18" si="8">F13*H13</f>
         <v>1</v>
       </c>
       <c r="N13">
-        <f>G13*H13</f>
+        <f t="shared" ref="N13:N18" si="9">G13*H13</f>
         <v>-1</v>
       </c>
       <c r="O13">
-        <f>I13*G13</f>
+        <f t="shared" ref="O13:O18" si="10">I13*G13</f>
         <v>-1</v>
       </c>
       <c r="P13">
-        <f>I13*H13</f>
+        <f t="shared" ref="P13:P18" si="11">I13*H13</f>
         <v>1</v>
       </c>
       <c r="Q13">
-        <f>J13*H13</f>
+        <f t="shared" ref="Q13:Q18" si="12">J13*H13</f>
         <v>-1</v>
       </c>
       <c r="R13">
-        <f>L13*H13</f>
+        <f t="shared" ref="R13:R18" si="13">L13*H13</f>
         <v>1</v>
       </c>
       <c r="S13">
-        <f>O13*H13</f>
+        <f t="shared" ref="S13:S18" si="14">O13*H13</f>
         <v>1</v>
       </c>
       <c r="T13">
@@ -1443,19 +1454,19 @@
         <v>0.69626792287366002</v>
       </c>
       <c r="W13">
-        <f>(T13+U13+V13)/3</f>
+        <f t="shared" si="0"/>
         <v>0.61898767912931663</v>
       </c>
       <c r="X13" s="2">
-        <f>T13-W13</f>
+        <f t="shared" si="1"/>
         <v>-5.9743981887266595E-2</v>
       </c>
       <c r="Y13" s="2">
-        <f>U13-W13</f>
+        <f t="shared" si="2"/>
         <v>-1.7536261857076574E-2</v>
       </c>
       <c r="Z13" s="2">
-        <f>V13-W13</f>
+        <f t="shared" si="3"/>
         <v>7.7280243744343391E-2</v>
       </c>
     </row>
@@ -1476,47 +1487,47 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <f>E14*F14</f>
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
       <c r="J14">
-        <f>E14*G14</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="K14">
-        <f>E14*H14</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L14">
-        <f>F14*G14</f>
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="M14">
-        <f>F14*H14</f>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
       <c r="N14">
-        <f>G14*H14</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O14">
-        <f>I14*G14</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="P14">
-        <f>I14*H14</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="Q14">
-        <f>J14*H14</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="R14">
-        <f>L14*H14</f>
+        <f t="shared" si="13"/>
         <v>-1</v>
       </c>
       <c r="S14">
-        <f>O14*H14</f>
+        <f t="shared" si="14"/>
         <v>-1</v>
       </c>
       <c r="T14">
@@ -1529,19 +1540,19 @@
         <v>1.2921968681019001E-2</v>
       </c>
       <c r="W14">
-        <f>(T14+U14+V14)/3</f>
+        <f t="shared" si="0"/>
         <v>1.3147546433018667E-2</v>
       </c>
       <c r="X14" s="2">
-        <f>T14-W14</f>
+        <f t="shared" si="1"/>
         <v>-2.2358960973266687E-4</v>
       </c>
       <c r="Y14" s="2">
-        <f>U14-W14</f>
+        <f t="shared" si="2"/>
         <v>4.491673617323319E-4</v>
       </c>
       <c r="Z14" s="2">
-        <f>V14-W14</f>
+        <f t="shared" si="3"/>
         <v>-2.2557775199966677E-4</v>
       </c>
     </row>
@@ -1562,47 +1573,47 @@
         <v>-1</v>
       </c>
       <c r="I15">
-        <f>E15*F15</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J15">
-        <f>E15*G15</f>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="K15">
-        <f>E15*H15</f>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="L15">
-        <f>F15*G15</f>
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="M15">
-        <f>F15*H15</f>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
       <c r="N15">
-        <f>G15*H15</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O15">
-        <f>I15*G15</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="P15">
-        <f>I15*H15</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="Q15">
-        <f>J15*H15</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="R15">
-        <f>L15*H15</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="S15">
-        <f>O15*H15</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T15">
@@ -1615,19 +1626,19 @@
         <v>7.8126374739168995E-3</v>
       </c>
       <c r="W15">
-        <f>(T15+U15+V15)/3</f>
+        <f t="shared" si="0"/>
         <v>7.8359718421951996E-3</v>
       </c>
       <c r="X15" s="2">
-        <f>T15-W15</f>
+        <f t="shared" si="1"/>
         <v>3.5938907375996504E-6</v>
       </c>
       <c r="Y15" s="2">
-        <f>U15-W15</f>
+        <f t="shared" si="2"/>
         <v>1.9740477540700421E-5</v>
       </c>
       <c r="Z15" s="2">
-        <f>V15-W15</f>
+        <f t="shared" si="3"/>
         <v>-2.3334368278300072E-5</v>
       </c>
     </row>
@@ -1648,47 +1659,47 @@
         <v>1</v>
       </c>
       <c r="I16">
-        <f>E16*F16</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J16">
-        <f>E16*G16</f>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="K16">
-        <f>E16*H16</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L16">
-        <f>F16*G16</f>
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
       <c r="M16">
-        <f>F16*H16</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="N16">
-        <f>G16*H16</f>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="O16">
-        <f>I16*G16</f>
+        <f t="shared" si="10"/>
         <v>-1</v>
       </c>
       <c r="P16">
-        <f>I16*H16</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="Q16">
-        <f>J16*H16</f>
+        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
       <c r="R16">
-        <f>L16*H16</f>
+        <f t="shared" si="13"/>
         <v>-1</v>
       </c>
       <c r="S16">
-        <f>O16*H16</f>
+        <f t="shared" si="14"/>
         <v>-1</v>
       </c>
       <c r="T16">
@@ -1701,19 +1712,19 @@
         <v>3.9139341313513001E-2</v>
       </c>
       <c r="W16">
-        <f>(T16+U16+V16)/3</f>
+        <f t="shared" si="0"/>
         <v>3.9443375408070004E-2</v>
       </c>
       <c r="X16" s="2">
-        <f>T16-W16</f>
+        <f t="shared" si="1"/>
         <v>-3.4579618663700684E-4</v>
       </c>
       <c r="Y16" s="2">
-        <f>U16-W16</f>
+        <f t="shared" si="2"/>
         <v>6.4983028119399572E-4</v>
       </c>
       <c r="Z16" s="2">
-        <f>V16-W16</f>
+        <f t="shared" si="3"/>
         <v>-3.0403409455700275E-4</v>
       </c>
     </row>
@@ -1734,47 +1745,47 @@
         <v>-1</v>
       </c>
       <c r="I17">
-        <f>E17*F17</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J17">
-        <f>E17*G17</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="K17">
-        <f>E17*H17</f>
+        <f t="shared" si="6"/>
         <v>-1</v>
       </c>
       <c r="L17">
-        <f>F17*G17</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="M17">
-        <f>F17*H17</f>
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
       <c r="N17">
-        <f>G17*H17</f>
+        <f t="shared" si="9"/>
         <v>-1</v>
       </c>
       <c r="O17">
-        <f>I17*G17</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P17">
-        <f>I17*H17</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
       <c r="Q17">
-        <f>J17*H17</f>
+        <f t="shared" si="12"/>
         <v>-1</v>
       </c>
       <c r="R17">
-        <f>L17*H17</f>
+        <f t="shared" si="13"/>
         <v>-1</v>
       </c>
       <c r="S17">
-        <f>O17*H17</f>
+        <f t="shared" si="14"/>
         <v>-1</v>
       </c>
       <c r="T17">
@@ -1787,19 +1798,19 @@
         <v>0.53561198577608005</v>
       </c>
       <c r="W17">
-        <f>(T17+U17+V17)/3</f>
+        <f t="shared" si="0"/>
         <v>0.60606291557457004</v>
       </c>
       <c r="X17" s="2">
-        <f>T17-W17</f>
+        <f t="shared" si="1"/>
         <v>-1.6982150968530063E-2</v>
       </c>
       <c r="Y17" s="2">
-        <f>U17-W17</f>
+        <f t="shared" si="2"/>
         <v>8.7433080767019944E-2</v>
       </c>
       <c r="Z17" s="2">
-        <f>V17-W17</f>
+        <f t="shared" si="3"/>
         <v>-7.0450929798489992E-2</v>
       </c>
     </row>
@@ -1820,47 +1831,47 @@
         <v>1</v>
       </c>
       <c r="I18">
-        <f>E18*F18</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J18">
-        <f>E18*G18</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="K18">
-        <f>E18*H18</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="L18">
-        <f>F18*G18</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="M18">
-        <f>F18*H18</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="N18">
-        <f>G18*H18</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="O18">
-        <f>I18*G18</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P18">
-        <f>I18*H18</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="Q18">
-        <f>J18*H18</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="R18">
-        <f>L18*H18</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="S18">
-        <f>O18*H18</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="T18">
@@ -1873,19 +1884,19 @@
         <v>8.1988133588322999E-3</v>
       </c>
       <c r="W18">
-        <f>(T18+U18+V18)/3</f>
+        <f t="shared" si="0"/>
         <v>8.1602334468118005E-3</v>
       </c>
       <c r="X18" s="2">
-        <f>T18-W18</f>
+        <f t="shared" si="1"/>
         <v>-4.2617098376600271E-5</v>
       </c>
       <c r="Y18" s="2">
-        <f>U18-W18</f>
+        <f t="shared" si="2"/>
         <v>4.0371863560990928E-6</v>
       </c>
       <c r="Z18" s="2">
-        <f>V18-W18</f>
+        <f t="shared" si="3"/>
         <v>3.8579912020499443E-5</v>
       </c>
     </row>
@@ -1966,7 +1977,7 @@
         <v>3.4551966404438389E-2</v>
       </c>
       <c r="Z20" s="2">
-        <f t="shared" ref="Y20:Z20" si="0">Z3+Z4+Z5+Z6+Z7+Z8+Z9+Z10+Z11+Z12+Z13+Z14+Z15+Z16+Z17+Z18</f>
+        <f t="shared" ref="Z20" si="15">Z3+Z4+Z5+Z6+Z7+Z8+Z9+Z10+Z11+Z12+Z13+Z14+Z15+Z16+Z17+Z18</f>
         <v>4.0066740858496736E-2</v>
       </c>
       <c r="AA20" t="s">
@@ -1982,63 +1993,63 @@
         <v>0.1768374304859833</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" ref="E21:S21" si="1">E20/16</f>
+        <f t="shared" ref="E21:S21" si="16">E20/16</f>
         <v>-7.277753170177927E-3</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>-4.1068236764515448E-3</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>0.1486514993668791</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>-0.14818769600927187</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>-7.7229571442067007E-5</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>-6.6215830367552121E-3</v>
       </c>
       <c r="K21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>6.5213112403576367E-3</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>3.2383998382866906E-4</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>-6.0705288298961736E-4</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>-0.16630864441764151</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>-6.1780587117341186E-4</v>
       </c>
       <c r="P21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>6.9961801143301864E-4</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>7.0393254805417287E-3</v>
       </c>
       <c r="R21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>1.6751275246558294E-3</v>
       </c>
       <c r="S21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="16"/>
         <v>2.1666998903570854E-4</v>
       </c>
       <c r="X21" s="2">
@@ -2046,11 +2057,11 @@
         <v>-4.6636692039334418E-3</v>
       </c>
       <c r="Y21" s="2">
-        <f t="shared" ref="Y21:Z21" si="2">Y20/16</f>
+        <f t="shared" ref="Y21:Z21" si="17">Y20/16</f>
         <v>2.1594979002773993E-3</v>
       </c>
       <c r="Z21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="17"/>
         <v>2.504171303656046E-3</v>
       </c>
       <c r="AA21" t="s">
@@ -2063,63 +2074,63 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2">
-        <f t="shared" ref="E22:S22" si="3">(E21^2)*16*3</f>
+        <f t="shared" ref="E22:S22" si="18">(E21^2)*16*3</f>
         <v>2.5423531778896733E-3</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>8.0956803405422318E-4</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>1.0606688766730206</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>1.0540604759297456</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>2.8629152184601594E-7</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>2.1045773718069301E-3</v>
       </c>
       <c r="K22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>2.0413200140935134E-3</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>5.0338720860553265E-6</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>1.7688633731808293E-5</v>
       </c>
       <c r="N22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>1.327611129985609</v>
       </c>
       <c r="O22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>1.8320836533904241E-5</v>
       </c>
       <c r="P22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>2.3494337372231587E-5</v>
       </c>
       <c r="Q22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>2.3785009546081941E-3</v>
       </c>
       <c r="R22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>1.3469050674525917E-4</v>
       </c>
       <c r="S22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="18"/>
         <v>2.2534024391392348E-6</v>
       </c>
       <c r="X22" s="2">
@@ -2139,62 +2150,65 @@
       </c>
     </row>
     <row r="23" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="E23">
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="3">
         <f>E22*100/Z25</f>
         <v>7.2615966843228977E-2</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <f>F22*100/Z25</f>
         <v>2.3123288310012546E-2</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="3">
         <f>G22*100/Z25</f>
         <v>30.295356542109573</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="3">
         <f>H22*100/Z25</f>
         <v>30.106604084963255</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="3">
         <v>0</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="3">
         <f>J22*100/Z25</f>
         <v>6.0111994658821541E-2</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="3">
         <f>K22*100/Z25</f>
         <v>5.8305206274636201E-2</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="3">
         <f>L22*100/Z25</f>
         <v>1.4377997977349166E-4</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="3">
         <f>M22*100/Z25</f>
         <v>5.0523163018492039E-4</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="3">
         <f>N22*100/Z25</f>
         <v>37.919895093316704</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="3">
         <f>O22*100/Z25</f>
         <v>5.2328892376413215E-4</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="3">
         <f>P22*100/Z25</f>
         <v>6.7105705000504836E-4</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="3">
         <f>Q22*100/Z25</f>
         <v>6.7935937445081529E-2</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="3">
         <f>R22*100/Z25</f>
         <v>3.8470978214089364E-3</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="3">
         <f>S22*100/Z25</f>
         <v>6.4362810890347075E-5</v>
       </c>
@@ -2207,9 +2221,12 @@
       </c>
     </row>
     <row r="24" spans="3:27" x14ac:dyDescent="0.3">
-      <c r="Z24" s="2">
+      <c r="Z24" s="3">
         <f>Z23*100/Z25</f>
         <v>1.3902888906605859</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="3:27" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Grafico brutto analisi fattoriale
</commit_message>
<xml_diff>
--- a/analysis/analisiFattoriale-tmkX/Factorial Analysis 3 repeat.xlsx
+++ b/analysis/analisiFattoriale-tmkX/Factorial Analysis 3 repeat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaia\Documents\GitHub\PECSNproject\analysis\analisiFattoriale-tmkX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clari\OneDrive\Desktop\Git\PECSNproject\analysis\analisiFattoriale-tmkX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DB04AB-9977-4111-AE71-36A49E1DEE04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C50C521-2FC9-4D7F-A72C-9AB03180475E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C7BA823-641E-4C67-8975-4763F16E04BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5C7BA823-641E-4C67-8975-4763F16E04BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -165,8 +165,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -194,13 +202,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -216,6 +225,1004 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1160255905511811"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.85341885389326333"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.2222222222222247E-2"/>
+                  <c:y val="0"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-1C1E-4F77-A385-08DB98AB7D80}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.1395942465319696E-2"/>
+                  <c:y val="-2.7777777777777776E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-1C1E-4F77-A385-08DB98AB7D80}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Foglio1!$E$25:$S$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>7.2615966843228975E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3123288310012547E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30295356542109575</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30106604084963257</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0111994658821537E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.8305206274636206E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4377997977349165E-6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.0523163018492035E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.37919895093316702</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.2328892376413218E-6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.7105705000504839E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.7935937445081534E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8470978214089364E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.4362810890347072E-7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1C1E-4F77-A385-08DB98AB7D80}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2030216208"/>
+        <c:axId val="2030230768"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2030216208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="@" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="94000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2030230768"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2030230768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2030216208"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>138110</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BCF75D1-C03C-480F-8A23-21349AD3E69D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -517,29 +1524,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641A5261-CE43-4139-AE63-77AF2ADD7BDE}">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="9.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.44140625" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>8</v>
       </c>
@@ -610,7 +1617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1</v>
       </c>
@@ -685,7 +1692,7 @@
         <v>-4.2407288846000452E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -763,7 +1770,7 @@
         <v>4.8169365857430035E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -841,7 +1848,7 @@
         <v>0.10457121213873677</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -919,7 +1926,7 @@
         <v>6.8057992421933361E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -997,7 +2004,7 @@
         <v>-3.2354694804302697E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>1</v>
       </c>
@@ -1072,7 +2079,7 @@
         <v>-5.2191837180933648E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>1</v>
       </c>
@@ -1147,7 +2154,7 @@
         <v>-7.3745141720623408E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1225,7 +2232,7 @@
         <v>-3.8085099772565412E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1303,7 +2310,7 @@
         <v>5.6513405562334806E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -1381,7 +2388,7 @@
         <v>-1.9935416629480035E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1470,7 +2477,7 @@
         <v>7.7280243744343391E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>1</v>
       </c>
@@ -1556,7 +2563,7 @@
         <v>-2.2557775199966677E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>1</v>
       </c>
@@ -1642,7 +2649,7 @@
         <v>-2.3334368278300072E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>1</v>
       </c>
@@ -1728,7 +2735,7 @@
         <v>-3.0403409455700275E-4</v>
       </c>
     </row>
-    <row r="17" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>1</v>
       </c>
@@ -1814,7 +2821,7 @@
         <v>-7.0450929798489992E-2</v>
       </c>
     </row>
-    <row r="18" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>1</v>
       </c>
@@ -1900,7 +2907,7 @@
         <v>3.8579912020499443E-5</v>
       </c>
     </row>
-    <row r="20" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>31</v>
       </c>
@@ -1984,7 +2991,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>32</v>
       </c>
@@ -2068,7 +3075,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>37</v>
       </c>
@@ -2149,7 +3156,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>39</v>
       </c>
@@ -2220,7 +3227,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:27" x14ac:dyDescent="0.25">
       <c r="Z24" s="3">
         <f>Z23*100/Z25</f>
         <v>1.3902888906605859</v>
@@ -2229,7 +3236,67 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f>E23/100</f>
+        <v>7.2615966843228975E-4</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25:S25" si="19">F23/100</f>
+        <v>2.3123288310012547E-4</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="19"/>
+        <v>0.30295356542109575</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="19"/>
+        <v>0.30106604084963257</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="19"/>
+        <v>6.0111994658821537E-4</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="19"/>
+        <v>5.8305206274636206E-4</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="19"/>
+        <v>1.4377997977349165E-6</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="19"/>
+        <v>5.0523163018492035E-6</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="19"/>
+        <v>0.37919895093316702</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="19"/>
+        <v>5.2328892376413218E-6</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="19"/>
+        <v>6.7105705000504839E-6</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="19"/>
+        <v>6.7935937445081534E-4</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="19"/>
+        <v>3.8470978214089364E-5</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="19"/>
+        <v>6.4362810890347072E-7</v>
+      </c>
       <c r="Z25" s="2">
         <f>E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22+Q22+R22+S22+Z23</f>
         <v>3.5010938894174255</v>
@@ -2238,11 +3305,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:27" x14ac:dyDescent="0.25">
       <c r="I27" s="2"/>
+      <c r="Q27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
immagini confronto response time
</commit_message>
<xml_diff>
--- a/analysis/analisiFattoriale-tmkX/Factorial Analysis 3 repeat.xlsx
+++ b/analysis/analisiFattoriale-tmkX/Factorial Analysis 3 repeat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Poggiani\Documents\GitHub\PECSNproject\analysis\analisiFattoriale-tmkX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CE0F10-7EE6-4BCB-ACDE-CC7C9FA90407}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFF2FFF-23FB-4645-8754-CCB0B7F5F24C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14016" yWindow="4176" windowWidth="21888" windowHeight="10044" xr2:uid="{5C7BA823-641E-4C67-8975-4763F16E04BA}"/>
+    <workbookView minimized="1" xWindow="744" yWindow="3072" windowWidth="21888" windowHeight="10044" xr2:uid="{5C7BA823-641E-4C67-8975-4763F16E04BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>t = ${0.5,2}s</t>
   </si>
@@ -240,11 +240,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,7 +722,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.0201443569553805E-2"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.65304790026246717"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1213,6 +1223,7 @@
         <c:crossAx val="1047307680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1047307680"/>
@@ -3996,10 +4007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641A5261-CE43-4139-AE63-77AF2ADD7BDE}">
-  <dimension ref="A1:AA95"/>
+  <dimension ref="A1:AA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W36" sqref="W36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5905,10 +5916,10 @@
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="5"/>
+      <c r="B44" s="7"/>
       <c r="V44">
         <v>0.58908076460603997</v>
       </c>
@@ -5933,16 +5944,16 @@
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="5" t="s">
         <v>44</v>
       </c>
       <c r="V47">
@@ -5963,7 +5974,7 @@
         <f>_xlfn.NORM.S.INV(D48)</f>
         <v>-2.3109913382574181</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="6">
         <f>(A48-0.5)/48</f>
         <v>1.0416666666666666E-2</v>
       </c>
@@ -5986,7 +5997,7 @@
         <f t="shared" ref="C49:C95" si="20">_xlfn.NORM.S.INV(D49)</f>
         <v>-1.8627318674216511</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="6">
         <f t="shared" ref="D49:D95" si="21">(A49-0.5)/48</f>
         <v>3.125E-2</v>
       </c>
@@ -6009,7 +6020,7 @@
         <f t="shared" si="20"/>
         <v>-1.6249807216131986</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="6">
         <f t="shared" si="21"/>
         <v>5.2083333333333336E-2</v>
       </c>
@@ -6032,7 +6043,7 @@
         <f t="shared" si="20"/>
         <v>-1.4544076028560404</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="6">
         <f t="shared" si="21"/>
         <v>7.2916666666666671E-2</v>
       </c>
@@ -6055,7 +6066,7 @@
         <f t="shared" si="20"/>
         <v>-1.3180108973035372</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="6">
         <f t="shared" si="21"/>
         <v>9.375E-2</v>
       </c>
@@ -6078,7 +6089,7 @@
         <f t="shared" si="20"/>
         <v>-1.2025082629254475</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="6">
         <f t="shared" si="21"/>
         <v>0.11458333333333333</v>
       </c>
@@ -6101,7 +6112,7 @@
         <f t="shared" si="20"/>
         <v>-1.1011455083738533</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D54" s="6">
         <f t="shared" si="21"/>
         <v>0.13541666666666666</v>
       </c>
@@ -6124,7 +6135,7 @@
         <f t="shared" si="20"/>
         <v>-1.0099901692495805</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D55" s="6">
         <f t="shared" si="21"/>
         <v>0.15625</v>
       </c>
@@ -6147,7 +6158,7 @@
         <f t="shared" si="20"/>
         <v>-0.92653759925502854</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D56" s="6">
         <f t="shared" si="21"/>
         <v>0.17708333333333334</v>
       </c>
@@ -6170,7 +6181,7 @@
         <f t="shared" si="20"/>
         <v>-0.84908619169171662</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="6">
         <f t="shared" si="21"/>
         <v>0.19791666666666666</v>
       </c>
@@ -6193,7 +6204,7 @@
         <f t="shared" si="20"/>
         <v>-0.77642176114792794</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="6">
         <f t="shared" si="21"/>
         <v>0.21875</v>
       </c>
@@ -6216,7 +6227,7 @@
         <f t="shared" si="20"/>
         <v>-0.70764350875288007</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="6">
         <f t="shared" si="21"/>
         <v>0.23958333333333334</v>
       </c>
@@ -6239,7 +6250,7 @@
         <f t="shared" si="20"/>
         <v>-0.64206137527650098</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="6">
         <f t="shared" si="21"/>
         <v>0.26041666666666669</v>
       </c>
@@ -6262,7 +6273,7 @@
         <f t="shared" si="20"/>
         <v>-0.57913216225555586</v>
       </c>
-      <c r="D61" s="7">
+      <c r="D61" s="6">
         <f t="shared" si="21"/>
         <v>0.28125</v>
       </c>
@@ -6285,7 +6296,7 @@
         <f t="shared" si="20"/>
         <v>-0.51841798843925346</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D62" s="6">
         <f t="shared" si="21"/>
         <v>0.30208333333333331</v>
       </c>
@@ -6308,7 +6319,7 @@
         <f t="shared" si="20"/>
         <v>-0.45955824853388244</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D63" s="6">
         <f t="shared" si="21"/>
         <v>0.32291666666666669</v>
       </c>
@@ -6331,7 +6342,7 @@
         <f t="shared" si="20"/>
         <v>-0.40225006532172536</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64" s="6">
         <f t="shared" si="21"/>
         <v>0.34375</v>
       </c>
@@ -6354,7 +6365,7 @@
         <f t="shared" si="20"/>
         <v>-0.34623426359988241</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D65" s="6">
         <f t="shared" si="21"/>
         <v>0.36458333333333331</v>
       </c>
@@ -6377,7 +6388,7 @@
         <f t="shared" si="20"/>
         <v>-0.29128503300340081</v>
       </c>
-      <c r="D66" s="7">
+      <c r="D66" s="6">
         <f t="shared" si="21"/>
         <v>0.38541666666666669</v>
       </c>
@@ -6400,7 +6411,7 @@
         <f t="shared" si="20"/>
         <v>-0.23720210932878771</v>
       </c>
-      <c r="D67" s="7">
+      <c r="D67" s="6">
         <f t="shared" si="21"/>
         <v>0.40625</v>
       </c>
@@ -6423,9 +6434,18 @@
         <f t="shared" si="20"/>
         <v>-0.18380470283773828</v>
       </c>
-      <c r="D68" s="7">
+      <c r="D68" s="6">
         <f t="shared" si="21"/>
         <v>0.42708333333333331</v>
+      </c>
+      <c r="H68" t="s">
+        <v>42</v>
+      </c>
+      <c r="I68" t="s">
+        <v>43</v>
+      </c>
+      <c r="J68" t="s">
+        <v>44</v>
       </c>
       <c r="V68">
         <v>0.59046036659578005</v>
@@ -6446,9 +6466,18 @@
         <f t="shared" si="20"/>
         <v>-0.13092664893666775</v>
       </c>
-      <c r="D69" s="7">
+      <c r="D69" s="6">
         <f t="shared" si="21"/>
         <v>0.44791666666666669</v>
+      </c>
+      <c r="H69">
+        <v>-7.3745141720623408E-2</v>
+      </c>
+      <c r="I69">
+        <v>-2.3109913382574181</v>
+      </c>
+      <c r="J69">
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="V69">
         <v>8.3570422034003004E-3</v>
@@ -6469,9 +6498,18 @@
         <f t="shared" si="20"/>
         <v>-7.8412412733112211E-2</v>
       </c>
-      <c r="D70" s="7">
+      <c r="D70" s="6">
         <f t="shared" si="21"/>
         <v>0.46875</v>
+      </c>
+      <c r="H70">
+        <v>-7.0450929798489992E-2</v>
+      </c>
+      <c r="I70">
+        <v>-1.8627318674216511</v>
+      </c>
+      <c r="J70">
+        <v>3.125E-2</v>
       </c>
       <c r="V70">
         <v>1.2074195198359E-2</v>
@@ -6492,9 +6530,18 @@
         <f t="shared" si="20"/>
         <v>-2.6113678815527799E-2</v>
       </c>
-      <c r="D71" s="7">
+      <c r="D71" s="6">
         <f t="shared" si="21"/>
         <v>0.48958333333333331</v>
+      </c>
+      <c r="H71">
+        <v>-6.0591280487763188E-2</v>
+      </c>
+      <c r="I71">
+        <v>-1.6249807216131986</v>
+      </c>
+      <c r="J71">
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="V71">
         <v>4.8828473236715998E-2</v>
@@ -6515,9 +6562,18 @@
         <f t="shared" si="20"/>
         <v>2.6113678815527657E-2</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D72" s="6">
         <f t="shared" si="21"/>
         <v>0.51041666666666663</v>
+      </c>
+      <c r="H72">
+        <v>-5.9743981887266595E-2</v>
+      </c>
+      <c r="I72">
+        <v>-1.4544076028560404</v>
+      </c>
+      <c r="J72">
+        <v>7.2916666666666671E-2</v>
       </c>
       <c r="V72">
         <v>0.69626792287366002</v>
@@ -6538,9 +6594,18 @@
         <f t="shared" si="20"/>
         <v>7.8412412733112211E-2</v>
       </c>
-      <c r="D73" s="7">
+      <c r="D73" s="6">
         <f t="shared" si="21"/>
         <v>0.53125</v>
+      </c>
+      <c r="H73">
+        <v>-4.3979931650973247E-2</v>
+      </c>
+      <c r="I73">
+        <v>-1.3180108973035372</v>
+      </c>
+      <c r="J73">
+        <v>9.375E-2</v>
       </c>
       <c r="V73">
         <v>1.2921968681019001E-2</v>
@@ -6561,9 +6626,18 @@
         <f t="shared" si="20"/>
         <v>0.13092664893666786</v>
       </c>
-      <c r="D74" s="7">
+      <c r="D74" s="6">
         <f t="shared" si="21"/>
         <v>0.55208333333333337</v>
+      </c>
+      <c r="H74">
+        <v>-1.7536261857076574E-2</v>
+      </c>
+      <c r="I74">
+        <v>-1.2025082629254475</v>
+      </c>
+      <c r="J74">
+        <v>0.11458333333333333</v>
       </c>
       <c r="V74">
         <v>7.8126374739168995E-3</v>
@@ -6584,9 +6658,18 @@
         <f t="shared" si="20"/>
         <v>0.18380470283773812</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D75" s="6">
         <f t="shared" si="21"/>
         <v>0.57291666666666663</v>
+      </c>
+      <c r="H75">
+        <v>-1.6982150968530063E-2</v>
+      </c>
+      <c r="I75">
+        <v>-1.1011455083738533</v>
+      </c>
+      <c r="J75">
+        <v>0.13541666666666666</v>
       </c>
       <c r="V75">
         <v>3.9139341313513001E-2</v>
@@ -6607,9 +6690,18 @@
         <f t="shared" si="20"/>
         <v>0.23720210932878771</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D76" s="6">
         <f t="shared" si="21"/>
         <v>0.59375</v>
+      </c>
+      <c r="H76">
+        <v>-5.7811488452519932E-3</v>
+      </c>
+      <c r="I76">
+        <v>-1.0099901692495805</v>
+      </c>
+      <c r="J76">
+        <v>0.15625</v>
       </c>
       <c r="V76">
         <v>0.53561198577608005</v>
@@ -6630,9 +6722,18 @@
         <f t="shared" si="20"/>
         <v>0.29128503300340097</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="6">
         <f t="shared" si="21"/>
         <v>0.61458333333333337</v>
+      </c>
+      <c r="H77">
+        <v>-1.9935416629480035E-3</v>
+      </c>
+      <c r="I77">
+        <v>-0.92653759925502854</v>
+      </c>
+      <c r="J77">
+        <v>0.17708333333333334</v>
       </c>
       <c r="V77">
         <v>8.1988133588322999E-3</v>
@@ -6653,9 +6754,18 @@
         <f t="shared" si="20"/>
         <v>0.3462342635998823</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D78" s="6">
         <f t="shared" si="21"/>
         <v>0.63541666666666663</v>
+      </c>
+      <c r="H78">
+        <v>-5.3892032117266661E-4</v>
+      </c>
+      <c r="I78">
+        <v>-0.84908619169171662</v>
+      </c>
+      <c r="J78">
+        <v>0.19791666666666666</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.3">
@@ -6670,9 +6780,18 @@
         <f t="shared" si="20"/>
         <v>0.40225006532172536</v>
       </c>
-      <c r="D79" s="7">
+      <c r="D79" s="6">
         <f t="shared" si="21"/>
         <v>0.65625</v>
+      </c>
+      <c r="H79">
+        <v>-5.2191837180933648E-4</v>
+      </c>
+      <c r="I79">
+        <v>-0.77642176114792794</v>
+      </c>
+      <c r="J79">
+        <v>0.21875</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.3">
@@ -6687,12 +6806,21 @@
         <f t="shared" si="20"/>
         <v>0.45955824853388255</v>
       </c>
-      <c r="D80" s="7">
+      <c r="D80" s="6">
         <f t="shared" si="21"/>
         <v>0.67708333333333337</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H80">
+        <v>-3.4579618663700684E-4</v>
+      </c>
+      <c r="I80">
+        <v>-0.70764350875288007</v>
+      </c>
+      <c r="J80">
+        <v>0.23958333333333334</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="22"/>
         <v>34</v>
@@ -6704,12 +6832,21 @@
         <f t="shared" si="20"/>
         <v>0.51841798843925324</v>
       </c>
-      <c r="D81" s="7">
+      <c r="D81" s="6">
         <f t="shared" si="21"/>
         <v>0.69791666666666663</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H81">
+        <v>-3.0403409455700275E-4</v>
+      </c>
+      <c r="I81">
+        <v>-0.64206137527650098</v>
+      </c>
+      <c r="J81">
+        <v>0.26041666666666669</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82">
         <f t="shared" si="22"/>
         <v>35</v>
@@ -6721,12 +6858,21 @@
         <f t="shared" si="20"/>
         <v>0.57913216225555586</v>
       </c>
-      <c r="D82" s="7">
+      <c r="D82" s="6">
         <f t="shared" si="21"/>
         <v>0.71875</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H82">
+        <v>-2.2557775199966677E-4</v>
+      </c>
+      <c r="I82">
+        <v>-0.57913216225555586</v>
+      </c>
+      <c r="J82">
+        <v>0.28125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="22"/>
         <v>36</v>
@@ -6738,12 +6884,21 @@
         <f t="shared" si="20"/>
         <v>0.64206137527650131</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D83" s="6">
         <f t="shared" si="21"/>
         <v>0.73958333333333337</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H83">
+        <v>-2.2358960973266687E-4</v>
+      </c>
+      <c r="I83">
+        <v>-0.51841798843925346</v>
+      </c>
+      <c r="J83">
+        <v>0.30208333333333331</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="22"/>
         <v>37</v>
@@ -6755,12 +6910,21 @@
         <f t="shared" si="20"/>
         <v>0.70764350875288007</v>
       </c>
-      <c r="D84" s="7">
+      <c r="D84" s="6">
         <f t="shared" si="21"/>
         <v>0.76041666666666663</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H84">
+        <v>-1.8474552562933871E-4</v>
+      </c>
+      <c r="I84">
+        <v>-0.45955824853388244</v>
+      </c>
+      <c r="J84">
+        <v>0.32291666666666669</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85">
         <f t="shared" si="22"/>
         <v>38</v>
@@ -6772,12 +6936,21 @@
         <f t="shared" si="20"/>
         <v>0.77642176114792794</v>
       </c>
-      <c r="D85" s="7">
+      <c r="D85" s="6">
         <f t="shared" si="21"/>
         <v>0.78125</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H85">
+        <v>-1.41659603046667E-4</v>
+      </c>
+      <c r="I85">
+        <v>-0.40225006532172536</v>
+      </c>
+      <c r="J85">
+        <v>0.34375</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="22"/>
         <v>39</v>
@@ -6789,12 +6962,21 @@
         <f t="shared" si="20"/>
         <v>0.84908619169171662</v>
       </c>
-      <c r="D86" s="7">
+      <c r="D86" s="6">
         <f t="shared" si="21"/>
         <v>0.80208333333333337</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H86">
+        <v>-5.2829773582665704E-5</v>
+      </c>
+      <c r="I86">
+        <v>-0.34623426359988241</v>
+      </c>
+      <c r="J86">
+        <v>0.36458333333333331</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="22"/>
         <v>40</v>
@@ -6806,12 +6988,21 @@
         <f t="shared" si="20"/>
         <v>0.92653759925502854</v>
       </c>
-      <c r="D87" s="7">
+      <c r="D87" s="6">
         <f t="shared" si="21"/>
         <v>0.82291666666666663</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H87">
+        <v>-4.2617098376600271E-5</v>
+      </c>
+      <c r="I87">
+        <v>-0.29128503300340081</v>
+      </c>
+      <c r="J87">
+        <v>0.38541666666666669</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="22"/>
         <v>41</v>
@@ -6823,12 +7014,21 @@
         <f t="shared" si="20"/>
         <v>1.0099901692495805</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D88" s="6">
         <f t="shared" si="21"/>
         <v>0.84375</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H88">
+        <v>-4.2407288846000452E-5</v>
+      </c>
+      <c r="I88">
+        <v>-0.23720210932878771</v>
+      </c>
+      <c r="J88">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89">
         <f t="shared" si="22"/>
         <v>42</v>
@@ -6840,12 +7040,21 @@
         <f t="shared" si="20"/>
         <v>1.1011455083738533</v>
       </c>
-      <c r="D89" s="7">
+      <c r="D89" s="6">
         <f t="shared" si="21"/>
         <v>0.86458333333333337</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H89">
+        <v>-3.8085099772565412E-5</v>
+      </c>
+      <c r="I89">
+        <v>-0.18380470283773828</v>
+      </c>
+      <c r="J89">
+        <v>0.42708333333333331</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="22"/>
         <v>43</v>
@@ -6857,12 +7066,21 @@
         <f t="shared" si="20"/>
         <v>1.2025082629254478</v>
       </c>
-      <c r="D90" s="7">
+      <c r="D90" s="6">
         <f t="shared" si="21"/>
         <v>0.88541666666666663</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H90">
+        <v>-3.2354694804302697E-5</v>
+      </c>
+      <c r="I90">
+        <v>-0.13092664893666775</v>
+      </c>
+      <c r="J90">
+        <v>0.44791666666666669</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="22"/>
         <v>44</v>
@@ -6874,12 +7092,21 @@
         <f t="shared" si="20"/>
         <v>1.3180108973035372</v>
       </c>
-      <c r="D91" s="7">
+      <c r="D91" s="6">
         <f t="shared" si="21"/>
         <v>0.90625</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H91">
+        <v>-2.3334368278300072E-5</v>
+      </c>
+      <c r="I91">
+        <v>-7.8412412733112211E-2</v>
+      </c>
+      <c r="J91">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92">
         <f t="shared" si="22"/>
         <v>45</v>
@@ -6891,12 +7118,21 @@
         <f t="shared" si="20"/>
         <v>1.4544076028560411</v>
       </c>
-      <c r="D92" s="7">
+      <c r="D92" s="6">
         <f t="shared" si="21"/>
         <v>0.92708333333333337</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H92">
+        <v>-3.683631979665633E-6</v>
+      </c>
+      <c r="I92">
+        <v>-2.6113678815527799E-2</v>
+      </c>
+      <c r="J92">
+        <v>0.48958333333333331</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="22"/>
         <v>46</v>
@@ -6908,12 +7144,21 @@
         <f t="shared" si="20"/>
         <v>1.6249807216131986</v>
       </c>
-      <c r="D93" s="7">
+      <c r="D93" s="6">
         <f t="shared" si="21"/>
         <v>0.94791666666666663</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H93">
+        <v>1.8289695803350159E-7</v>
+      </c>
+      <c r="I93">
+        <v>2.6113678815527657E-2</v>
+      </c>
+      <c r="J93">
+        <v>0.51041666666666663</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="22"/>
         <v>47</v>
@@ -6925,12 +7170,21 @@
         <f t="shared" si="20"/>
         <v>1.8627318674216511</v>
       </c>
-      <c r="D94" s="7">
+      <c r="D94" s="6">
         <f t="shared" si="21"/>
         <v>0.96875</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H94">
+        <v>3.5938907375996504E-6</v>
+      </c>
+      <c r="I94">
+        <v>7.8412412733112211E-2</v>
+      </c>
+      <c r="J94">
+        <v>0.53125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="22"/>
         <v>48</v>
@@ -6942,8 +7196,248 @@
         <f t="shared" si="20"/>
         <v>2.3109913382574203</v>
       </c>
-      <c r="D95" s="7">
+      <c r="D95" s="6">
         <f t="shared" si="21"/>
+        <v>0.98958333333333337</v>
+      </c>
+      <c r="H95">
+        <v>4.0371863560990928E-6</v>
+      </c>
+      <c r="I95">
+        <v>0.13092664893666786</v>
+      </c>
+      <c r="J95">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H96">
+        <v>6.6767414870008701E-6</v>
+      </c>
+      <c r="I96">
+        <v>0.18380470283773812</v>
+      </c>
+      <c r="J96">
+        <v>0.57291666666666663</v>
+      </c>
+    </row>
+    <row r="97" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H97">
+        <v>1.0076710344598602E-5</v>
+      </c>
+      <c r="I97">
+        <v>0.23720210932878771</v>
+      </c>
+      <c r="J97">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="98" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H98">
+        <v>1.9740477540700421E-5</v>
+      </c>
+      <c r="I98">
+        <v>0.29128503300340097</v>
+      </c>
+      <c r="J98">
+        <v>0.61458333333333337</v>
+      </c>
+    </row>
+    <row r="99" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H99">
+        <v>2.2277984459698891E-5</v>
+      </c>
+      <c r="I99">
+        <v>0.3462342635998823</v>
+      </c>
+      <c r="J99">
+        <v>0.63541666666666663</v>
+      </c>
+    </row>
+    <row r="100" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H100">
+        <v>3.5730547358999581E-5</v>
+      </c>
+      <c r="I100">
+        <v>0.40225006532172536</v>
+      </c>
+      <c r="J100">
+        <v>0.65625</v>
+      </c>
+    </row>
+    <row r="101" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H101">
+        <v>3.7902202814533645E-5</v>
+      </c>
+      <c r="I101">
+        <v>0.45955824853388255</v>
+      </c>
+      <c r="J101">
+        <v>0.67708333333333337</v>
+      </c>
+    </row>
+    <row r="102" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H102">
+        <v>3.8579912020499443E-5</v>
+      </c>
+      <c r="I102">
+        <v>0.51841798843925324</v>
+      </c>
+      <c r="J102">
+        <v>0.69791666666666663</v>
+      </c>
+    </row>
+    <row r="103" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H103">
+        <v>5.6513405562334806E-5</v>
+      </c>
+      <c r="I103">
+        <v>0.57913216225555586</v>
+      </c>
+      <c r="J103">
+        <v>0.71875</v>
+      </c>
+    </row>
+    <row r="104" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H104">
+        <v>4.491673617323319E-4</v>
+      </c>
+      <c r="I104">
+        <v>0.64206137527650131</v>
+      </c>
+      <c r="J104">
+        <v>0.73958333333333337</v>
+      </c>
+    </row>
+    <row r="105" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H105">
+        <v>6.4983028119399572E-4</v>
+      </c>
+      <c r="I105">
+        <v>0.70764350875288007</v>
+      </c>
+      <c r="J105">
+        <v>0.76041666666666663</v>
+      </c>
+    </row>
+    <row r="106" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H106">
+        <v>6.8057992421933361E-4</v>
+      </c>
+      <c r="I106">
+        <v>0.77642176114792794</v>
+      </c>
+      <c r="J106">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="107" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H107">
+        <v>7.0666389743866131E-4</v>
+      </c>
+      <c r="I107">
+        <v>0.84908619169171662</v>
+      </c>
+      <c r="J107">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="108" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H108">
+        <v>7.5099874702599934E-4</v>
+      </c>
+      <c r="I108">
+        <v>0.92653759925502854</v>
+      </c>
+      <c r="J108">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="109" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H109">
+        <v>9.6421225950900358E-4</v>
+      </c>
+      <c r="I109">
+        <v>1.0099901692495805</v>
+      </c>
+      <c r="J109">
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="110" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H110">
+        <v>1.2425429159219972E-3</v>
+      </c>
+      <c r="I110">
+        <v>1.1011455083738533</v>
+      </c>
+      <c r="J110">
+        <v>0.86458333333333337</v>
+      </c>
+    </row>
+    <row r="111" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H111">
+        <v>4.8169365857430035E-3</v>
+      </c>
+      <c r="I111">
+        <v>1.2025082629254478</v>
+      </c>
+      <c r="J111">
+        <v>0.88541666666666663</v>
+      </c>
+    </row>
+    <row r="112" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H112">
+        <v>1.2731494653726583E-2</v>
+      </c>
+      <c r="I112">
+        <v>1.3180108973035372</v>
+      </c>
+      <c r="J112">
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="113" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H113">
+        <v>6.1013647066896493E-2</v>
+      </c>
+      <c r="I113">
+        <v>1.4544076028560411</v>
+      </c>
+      <c r="J113">
+        <v>0.92708333333333337</v>
+      </c>
+    </row>
+    <row r="114" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H114">
+        <v>7.7280243744343391E-2</v>
+      </c>
+      <c r="I114">
+        <v>1.6249807216131986</v>
+      </c>
+      <c r="J114">
+        <v>0.94791666666666663</v>
+      </c>
+    </row>
+    <row r="115" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H115">
+        <v>8.7433080767019944E-2</v>
+      </c>
+      <c r="I115">
+        <v>1.8627318674216511</v>
+      </c>
+      <c r="J115">
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="116" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H116">
+        <v>0.10457121213873677</v>
+      </c>
+      <c r="I116">
+        <v>2.3109913382574203</v>
+      </c>
+      <c r="J116">
         <v>0.98958333333333337</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cartella per experiment 2
</commit_message>
<xml_diff>
--- a/analysis/analisiFattoriale-tmkX/Factorial Analysis 3 repeat.xlsx
+++ b/analysis/analisiFattoriale-tmkX/Factorial Analysis 3 repeat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Poggiani\Documents\GitHub\PECSNproject\analysis\analisiFattoriale-tmkX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clari\Desktop\Git\PECSNproject\analysis\analisiFattoriale-tmkX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFF2FFF-23FB-4645-8754-CCB0B7F5F24C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F84EEA3-3309-47FF-86C5-3A1DB58785F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="744" yWindow="3072" windowWidth="21888" windowHeight="10044" xr2:uid="{5C7BA823-641E-4C67-8975-4763F16E04BA}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7875" xr2:uid="{5C7BA823-641E-4C67-8975-4763F16E04BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>t = ${0.5,2}s</t>
   </si>
@@ -175,6 +175,15 @@
   <si>
     <t>e</t>
   </si>
+  <si>
+    <t>New!!!</t>
+  </si>
+  <si>
+    <t>X = ${0.05, 2}s</t>
+  </si>
+  <si>
+    <t>m = ${0.5, 10}s</t>
+  </si>
 </sst>
 </file>
 
@@ -183,7 +192,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +213,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -232,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -245,9 +261,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -265,7 +282,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -302,7 +319,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -405,7 +422,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -562,7 +579,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2030230768"/>
@@ -624,7 +641,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2030216208"/>
@@ -665,7 +682,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -679,7 +696,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -716,7 +733,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -833,7 +850,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="it-IT"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1217,7 +1234,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1047307680"/>
@@ -1280,7 +1297,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1047307264"/>
@@ -1322,7 +1339,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1352,7 +1369,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1366,7 +1383,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1403,7 +1420,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1828,7 +1845,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="938956736"/>
@@ -1890,7 +1907,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="938953824"/>
@@ -1931,7 +1948,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3711,7 +3728,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4009,30 +4026,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641A5261-CE43-4139-AE63-77AF2ADD7BDE}">
   <dimension ref="A1:AA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W36" sqref="W36"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
-    <col min="5" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="9.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.44140625" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>8</v>
       </c>
@@ -4103,7 +4120,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="D3">
         <v>1</v>
       </c>
@@ -4178,8 +4198,11 @@
         <v>-4.2407288846000452E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="D4">
@@ -4256,8 +4279,11 @@
         <v>4.8169365857430035E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
@@ -4334,9 +4360,12 @@
         <v>0.10457121213873677</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -4412,9 +4441,12 @@
         <v>6.8057992421933361E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -4490,7 +4522,7 @@
         <v>-3.2354694804302697E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>1</v>
       </c>
@@ -4565,7 +4597,7 @@
         <v>-5.2191837180933648E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>1</v>
       </c>
@@ -4640,7 +4672,7 @@
         <v>-7.3745141720623408E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4718,7 +4750,7 @@
         <v>-3.8085099772565412E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -4796,7 +4828,7 @@
         <v>5.6513405562334806E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -4874,7 +4906,7 @@
         <v>-1.9935416629480035E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -4963,7 +4995,7 @@
         <v>7.7280243744343391E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>1</v>
       </c>
@@ -5049,7 +5081,7 @@
         <v>-2.2557775199966677E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>1</v>
       </c>
@@ -5135,7 +5167,7 @@
         <v>-2.3334368278300072E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>1</v>
       </c>
@@ -5221,7 +5253,7 @@
         <v>-3.0403409455700275E-4</v>
       </c>
     </row>
-    <row r="17" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>1</v>
       </c>
@@ -5307,7 +5339,7 @@
         <v>-7.0450929798489992E-2</v>
       </c>
     </row>
-    <row r="18" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:27" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>1</v>
       </c>
@@ -5393,7 +5425,7 @@
         <v>3.8579912020499443E-5</v>
       </c>
     </row>
-    <row r="20" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>31</v>
       </c>
@@ -5477,7 +5509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>32</v>
       </c>
@@ -5561,7 +5593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>37</v>
       </c>
@@ -5642,7 +5674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>39</v>
       </c>
@@ -5713,7 +5745,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:27" x14ac:dyDescent="0.25">
       <c r="Z24" s="3">
         <f>Z23*100/Z25</f>
         <v>1.3902888906605859</v>
@@ -5722,7 +5754,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E25">
         <f>E23/100</f>
         <v>7.2615966843228975E-4</v>
@@ -5791,11 +5823,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:27" x14ac:dyDescent="0.25">
       <c r="I27" s="2"/>
       <c r="Q27" s="4"/>
     </row>
-    <row r="29" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:27" x14ac:dyDescent="0.25">
       <c r="V29" t="s">
         <v>45</v>
       </c>
@@ -5803,7 +5835,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:27" x14ac:dyDescent="0.25">
       <c r="V30">
         <v>1.2415926875429001E-2</v>
       </c>
@@ -5811,7 +5843,7 @@
         <v>6.6767414870008701E-6</v>
       </c>
     </row>
-    <row r="31" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:27" x14ac:dyDescent="0.25">
       <c r="V31">
         <v>5.6181644550643998E-2</v>
       </c>
@@ -5819,7 +5851,7 @@
         <v>9.6421225950900358E-4</v>
       </c>
     </row>
-    <row r="32" spans="3:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:27" x14ac:dyDescent="0.25">
       <c r="V32">
         <v>0.61009369761105003</v>
       </c>
@@ -5827,7 +5859,7 @@
         <v>-6.0591280487763188E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V33" s="2">
         <v>1.4125790917746E-2</v>
       </c>
@@ -5835,7 +5867,7 @@
         <v>-1.41659603046667E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V34">
         <v>8.0071037843490005E-3</v>
       </c>
@@ -5843,7 +5875,7 @@
         <v>1.0076710344598602E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V35">
         <v>4.0451359408464997E-2</v>
       </c>
@@ -5851,7 +5883,7 @@
         <v>7.0666389743866131E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V36">
         <v>0.72521915538329995</v>
       </c>
@@ -5859,7 +5891,7 @@
         <v>6.1013647066896493E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V37">
         <v>8.3953102001308993E-3</v>
       </c>
@@ -5867,7 +5899,7 @@
         <v>1.8289695803350159E-7</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V38">
         <v>1.2013998160817E-2</v>
       </c>
@@ -5875,7 +5907,7 @@
         <v>-3.683631979665633E-6</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V39">
         <v>5.1573013646690001E-2</v>
       </c>
@@ -5883,7 +5915,7 @@
         <v>7.5099874702599934E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V40">
         <v>0.55924369724205003</v>
       </c>
@@ -5891,7 +5923,7 @@
         <v>-5.9743981887266595E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V41">
         <v>1.2923956823286E-2</v>
       </c>
@@ -5899,7 +5931,7 @@
         <v>-2.2358960973266687E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V42">
         <v>7.8395657329327992E-3</v>
       </c>
@@ -5907,7 +5939,7 @@
         <v>3.5938907375996504E-6</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V43">
         <v>3.9097579221432997E-2</v>
       </c>
@@ -5915,7 +5947,7 @@
         <v>-3.4579618663700684E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>41</v>
       </c>
@@ -5927,7 +5959,7 @@
         <v>-1.6982150968530063E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V45">
         <v>8.1176163484352002E-3</v>
       </c>
@@ -5935,7 +5967,7 @@
         <v>-4.2617098376600271E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V46">
         <v>1.2444980681301E-2</v>
       </c>
@@ -5943,7 +5975,7 @@
         <v>3.5730547358999581E-5</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>8</v>
       </c>
@@ -5963,7 +5995,7 @@
         <v>-5.7811488452519932E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -5985,7 +6017,7 @@
         <v>-4.3979931650973247E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49">
         <f>A48+1</f>
         <v>2</v>
@@ -6008,7 +6040,7 @@
         <v>-5.3892032117266661E-4</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" ref="A50:A95" si="22">A49+1</f>
         <v>3</v>
@@ -6031,7 +6063,7 @@
         <v>2.2277984459698891E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="22"/>
         <v>4</v>
@@ -6054,7 +6086,7 @@
         <v>-1.8474552562933871E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="22"/>
         <v>5</v>
@@ -6077,7 +6109,7 @@
         <v>1.2731494653726583E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="22"/>
         <v>6</v>
@@ -6100,7 +6132,7 @@
         <v>3.7902202814533645E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="22"/>
         <v>7</v>
@@ -6123,7 +6155,7 @@
         <v>-5.2829773582665704E-5</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="22"/>
         <v>8</v>
@@ -6146,7 +6178,7 @@
         <v>1.2425429159219972E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="22"/>
         <v>9</v>
@@ -6169,7 +6201,7 @@
         <v>-1.7536261857076574E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="22"/>
         <v>10</v>
@@ -6192,7 +6224,7 @@
         <v>4.491673617323319E-4</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="22"/>
         <v>11</v>
@@ -6215,7 +6247,7 @@
         <v>1.9740477540700421E-5</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="22"/>
         <v>12</v>
@@ -6238,7 +6270,7 @@
         <v>6.4983028119399572E-4</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="22"/>
         <v>13</v>
@@ -6261,7 +6293,7 @@
         <v>8.7433080767019944E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="22"/>
         <v>14</v>
@@ -6284,7 +6316,7 @@
         <v>4.0371863560990928E-6</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="22"/>
         <v>15</v>
@@ -6307,7 +6339,7 @@
         <v>-4.2407288846000452E-5</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="22"/>
         <v>16</v>
@@ -6330,7 +6362,7 @@
         <v>4.8169365857430035E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="22"/>
         <v>17</v>
@@ -6353,7 +6385,7 @@
         <v>0.10457121213873677</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="22"/>
         <v>18</v>
@@ -6376,7 +6408,7 @@
         <v>6.8057992421933361E-4</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="22"/>
         <v>19</v>
@@ -6399,7 +6431,7 @@
         <v>-3.2354694804302697E-5</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="22"/>
         <v>20</v>
@@ -6422,7 +6454,7 @@
         <v>-5.2191837180933648E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="22"/>
         <v>21</v>
@@ -6454,7 +6486,7 @@
         <v>-7.3745141720623408E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="22"/>
         <v>22</v>
@@ -6486,7 +6518,7 @@
         <v>-3.8085099772565412E-5</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="22"/>
         <v>23</v>
@@ -6518,7 +6550,7 @@
         <v>5.6513405562334806E-5</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="22"/>
         <v>24</v>
@@ -6550,7 +6582,7 @@
         <v>-1.9935416629480035E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="22"/>
         <v>25</v>
@@ -6582,7 +6614,7 @@
         <v>7.7280243744343391E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="22"/>
         <v>26</v>
@@ -6614,7 +6646,7 @@
         <v>-2.2557775199966677E-4</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="22"/>
         <v>27</v>
@@ -6646,7 +6678,7 @@
         <v>-2.3334368278300072E-5</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="22"/>
         <v>28</v>
@@ -6678,7 +6710,7 @@
         <v>-3.0403409455700275E-4</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="22"/>
         <v>29</v>
@@ -6710,7 +6742,7 @@
         <v>-7.0450929798489992E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="22"/>
         <v>30</v>
@@ -6742,7 +6774,7 @@
         <v>3.8579912020499403E-5</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="22"/>
         <v>31</v>
@@ -6768,7 +6800,7 @@
         <v>0.19791666666666666</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="22"/>
         <v>32</v>
@@ -6794,7 +6826,7 @@
         <v>0.21875</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="22"/>
         <v>33</v>
@@ -6820,7 +6852,7 @@
         <v>0.23958333333333334</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="22"/>
         <v>34</v>
@@ -6846,7 +6878,7 @@
         <v>0.26041666666666669</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="22"/>
         <v>35</v>
@@ -6872,7 +6904,7 @@
         <v>0.28125</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="22"/>
         <v>36</v>
@@ -6898,7 +6930,7 @@
         <v>0.30208333333333331</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="22"/>
         <v>37</v>
@@ -6924,7 +6956,7 @@
         <v>0.32291666666666669</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="22"/>
         <v>38</v>
@@ -6950,7 +6982,7 @@
         <v>0.34375</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="22"/>
         <v>39</v>
@@ -6976,7 +7008,7 @@
         <v>0.36458333333333331</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="22"/>
         <v>40</v>
@@ -7002,7 +7034,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="22"/>
         <v>41</v>
@@ -7028,7 +7060,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="22"/>
         <v>42</v>
@@ -7054,7 +7086,7 @@
         <v>0.42708333333333331</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="22"/>
         <v>43</v>
@@ -7080,7 +7112,7 @@
         <v>0.44791666666666669</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="22"/>
         <v>44</v>
@@ -7106,7 +7138,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="22"/>
         <v>45</v>
@@ -7132,7 +7164,7 @@
         <v>0.48958333333333331</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="22"/>
         <v>46</v>
@@ -7158,7 +7190,7 @@
         <v>0.51041666666666663</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="22"/>
         <v>47</v>
@@ -7184,7 +7216,7 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="22"/>
         <v>48</v>
@@ -7210,7 +7242,7 @@
         <v>0.55208333333333337</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H96">
         <v>6.6767414870008701E-6</v>
       </c>
@@ -7221,7 +7253,7 @@
         <v>0.57291666666666663</v>
       </c>
     </row>
-    <row r="97" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H97">
         <v>1.0076710344598602E-5</v>
       </c>
@@ -7232,7 +7264,7 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="98" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H98">
         <v>1.9740477540700421E-5</v>
       </c>
@@ -7243,7 +7275,7 @@
         <v>0.61458333333333337</v>
       </c>
     </row>
-    <row r="99" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H99">
         <v>2.2277984459698891E-5</v>
       </c>
@@ -7254,7 +7286,7 @@
         <v>0.63541666666666663</v>
       </c>
     </row>
-    <row r="100" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H100">
         <v>3.5730547358999581E-5</v>
       </c>
@@ -7265,7 +7297,7 @@
         <v>0.65625</v>
       </c>
     </row>
-    <row r="101" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H101">
         <v>3.7902202814533645E-5</v>
       </c>
@@ -7276,7 +7308,7 @@
         <v>0.67708333333333337</v>
       </c>
     </row>
-    <row r="102" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H102">
         <v>3.8579912020499443E-5</v>
       </c>
@@ -7287,7 +7319,7 @@
         <v>0.69791666666666663</v>
       </c>
     </row>
-    <row r="103" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H103">
         <v>5.6513405562334806E-5</v>
       </c>
@@ -7298,7 +7330,7 @@
         <v>0.71875</v>
       </c>
     </row>
-    <row r="104" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H104">
         <v>4.491673617323319E-4</v>
       </c>
@@ -7309,7 +7341,7 @@
         <v>0.73958333333333337</v>
       </c>
     </row>
-    <row r="105" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H105">
         <v>6.4983028119399572E-4</v>
       </c>
@@ -7320,7 +7352,7 @@
         <v>0.76041666666666663</v>
       </c>
     </row>
-    <row r="106" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H106">
         <v>6.8057992421933361E-4</v>
       </c>
@@ -7331,7 +7363,7 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="107" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H107">
         <v>7.0666389743866131E-4</v>
       </c>
@@ -7342,7 +7374,7 @@
         <v>0.80208333333333337</v>
       </c>
     </row>
-    <row r="108" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H108">
         <v>7.5099874702599934E-4</v>
       </c>
@@ -7353,7 +7385,7 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
-    <row r="109" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H109">
         <v>9.6421225950900358E-4</v>
       </c>
@@ -7364,7 +7396,7 @@
         <v>0.84375</v>
       </c>
     </row>
-    <row r="110" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H110">
         <v>1.2425429159219972E-3</v>
       </c>
@@ -7375,7 +7407,7 @@
         <v>0.86458333333333337</v>
       </c>
     </row>
-    <row r="111" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H111">
         <v>4.8169365857430035E-3</v>
       </c>
@@ -7386,7 +7418,7 @@
         <v>0.88541666666666663</v>
       </c>
     </row>
-    <row r="112" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H112">
         <v>1.2731494653726583E-2</v>
       </c>
@@ -7397,7 +7429,7 @@
         <v>0.90625</v>
       </c>
     </row>
-    <row r="113" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H113">
         <v>6.1013647066896493E-2</v>
       </c>
@@ -7408,7 +7440,7 @@
         <v>0.92708333333333337</v>
       </c>
     </row>
-    <row r="114" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H114">
         <v>7.7280243744343391E-2</v>
       </c>
@@ -7419,7 +7451,7 @@
         <v>0.94791666666666663</v>
       </c>
     </row>
-    <row r="115" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H115">
         <v>8.7433080767019944E-2</v>
       </c>
@@ -7430,7 +7462,7 @@
         <v>0.96875</v>
       </c>
     </row>
-    <row r="116" spans="8:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="8:10" x14ac:dyDescent="0.25">
       <c r="H116">
         <v>0.10457121213873677</v>
       </c>

</xml_diff>